<commit_message>
Closed all open issues
1. added jumper for voltage source
2. changed pin headers to 2 row dpdt switch
3. Changed VGA to correct footprint
4. Fixed placement of headphone jack
5. Converted BOM to csv
6. updated license file.
</commit_message>
<xml_diff>
--- a/BOM/SCART2VGA BOM.xlsx
+++ b/BOM/SCART2VGA BOM.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9321FC0-4166-4C18-8330-BEA687B74162}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raque\Documents\GitHub\SCART-to-VGA\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AFAF74-3ADF-404A-AC77-3B46985A5002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>Qty</t>
   </si>
@@ -172,18 +177,6 @@
     <t>https://console5.com/store/female-scart-jp21-through-hole-pcb-mount-21-pin-connector-right-angle.html</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>1x3</t>
-  </si>
-  <si>
-    <t>2.54mm</t>
-  </si>
-  <si>
-    <t>male pin headers</t>
-  </si>
-  <si>
     <t>J3</t>
   </si>
   <si>
@@ -233,24 +226,43 @@
   </si>
   <si>
     <t>https://www.arrow.com/en/products/sj1-3523ng/cui-inc</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>DPDT</t>
+  </si>
+  <si>
+    <t>THT RA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/c-k/JS202011AQN/401-2000-ND/1640096</t>
+  </si>
+  <si>
+    <t>https://www.arrow.com/en/products/js202011aqn/ck</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Toggle-Switches_C-K_JS202011AQN_C-K-JS202011AQN_C221662.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/D-Sub-Connectors_BOOMELE-Boom-Precision-Elec-VGA-002_C138387.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Audio-Video-Connectors_BOOMELE-Boom-Precision-Elec-PJ-307C_C16684.html</t>
+  </si>
+  <si>
+    <t>https://lcsc.com/product-detail/Interface-Specialized_HGSEMI-LM1881M-TR_C518922.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -273,20 +285,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,19 +609,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +631,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -645,7 +653,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -655,13 +663,13 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H2" t="s">
@@ -670,11 +678,8 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -684,7 +689,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
@@ -699,11 +704,8 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -713,7 +715,7 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" t="s">
@@ -728,11 +730,8 @@
       <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -742,26 +741,20 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>0.01</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -771,7 +764,7 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
@@ -786,11 +779,8 @@
       <c r="I6" t="s">
         <v>39</v>
       </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -800,24 +790,24 @@
       <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="4"/>
+      <c r="I7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="3"/>
       <c r="K7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -827,17 +817,14 @@
       <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -847,112 +834,101 @@
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
         <v>51</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="H9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="J10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="H10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="F11" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="G11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="G12" t="s">
         <v>69</v>
       </c>
+      <c r="H12" t="s">
+        <v>70</v>
+      </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H12" r:id="rId1" xr:uid="{3670C178-0AFA-4B7C-8F0D-041818D272A9}"/>
-    <hyperlink ref="G12" r:id="rId2" xr:uid="{A800B4CA-114E-4397-9FB3-57D7642B2E1A}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{C2CB1628-716F-443C-B08B-62D8B04C2933}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{EB44A1E2-E640-4B91-AED2-F2792B1297D2}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{1CF055A5-C23E-4718-A857-C4DEC6C67F49}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{8FEDD109-B07D-4010-8816-9DDD798D212C}"/>
-    <hyperlink ref="G11" r:id="rId7" xr:uid="{78C99112-7F83-4DB0-900B-7BB0CB91CAD5}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{F7621EDE-299B-4C2D-B5E3-7D2E41045E41}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>